<commit_message>
Se actualiza ventana de ventas
</commit_message>
<xml_diff>
--- a/ventas_dia.xlsx
+++ b/ventas_dia.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,18 +455,18 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>226</v>
+        <v>288</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Atun Pan En Aceite 150 GR</t>
+          <t>Cocacola</t>
         </is>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>5990</v>
+        <v>8330</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -475,24 +475,24 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-07-16 01:21:40</t>
+          <t>2025-08-07 14:59:26</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>227</v>
+        <v>289</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">LEVAPAN </t>
+          <t>Cocacola</t>
         </is>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>1785</v>
+        <v>8330</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -501,227 +501,45 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-07-16 01:28:01</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>228</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LEVAPAN </t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1785</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>efectivo</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2025-07-16 01:29:44</t>
+          <t>2025-08-07 15:00:50</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>229</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>SPAGEHETTI</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" t="n">
-        <v>4969.44</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>efectivo</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2025-07-16 01:36:53</t>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Resumen del Día</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>230</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>QUAKER SIN GLUTEN</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" t="n">
-        <v>3570</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>efectivo</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>2025-07-16 01:38:34</t>
-        </is>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Total Vendido</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>16660</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>231</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>FIBER PRO CLEAN 450g</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" t="n">
-        <v>15000</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>efectivo</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>2025-07-16 01:50:36</t>
-        </is>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Productos Vendidos</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>232</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Desodorante Gillette Hidra Gel Aloe Barras De 45g</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" t="n">
-        <v>10544</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>efectivo</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>2025-07-16 01:50:36</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>233</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>QUINUA ANCESTRAL EN HOJUELAS</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" t="n">
-        <v>4165</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>efectivo</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>2025-07-16 01:51:38</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>235</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Cocacola</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" t="n">
-        <v>8330</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Daviplata</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>2025-07-16 08:01:11</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Resumen del Día</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Total Vendido</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>56138.44</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Productos Vendidos</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A8" t="inlineStr">
         <is>
           <t>Número de Ventas</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>9</v>
+      <c r="B8" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>